<commit_message>
test(app): fix issue related to test_analyze_tc_1
</commit_message>
<xml_diff>
--- a/system_tests/data/analyze_tc_1/stories.xlsx
+++ b/system_tests/data/analyze_tc_1/stories.xlsx
@@ -11,10 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="3">
-  <si>
-    <t>Tabella 1</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="2">
   <si>
     <t>User Story</t>
   </si>
@@ -29,7 +26,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="4">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -41,15 +38,20 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <b val="1"/>
-      <sz val="10"/>
+      <sz val="15"/>
       <color indexed="8"/>
-      <name val="Helvetica Neue"/>
+      <name val="Calibri"/>
     </font>
     <font>
       <sz val="10"/>
       <color indexed="8"/>
       <name val="Arial"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="10"/>
+      <color indexed="8"/>
+      <name val="Helvetica Neue"/>
     </font>
   </fonts>
   <fills count="4">
@@ -72,7 +74,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="6">
+  <borders count="4">
     <border>
       <left/>
       <right/>
@@ -97,7 +99,7 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
@@ -106,52 +108,22 @@
         <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="11"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </left>
       <right style="thin">
         <color indexed="11"/>
       </right>
       <top style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </top>
       <bottom style="thin">
-        <color indexed="10"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
-        <color indexed="11"/>
-      </left>
-      <right style="thin">
-        <color indexed="10"/>
-      </right>
-      <top style="thin">
-        <color indexed="10"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="10"/>
+        <color indexed="13"/>
       </bottom>
       <diagonal/>
     </border>
@@ -161,32 +133,20 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="4" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" borderId="5" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -206,10 +166,11 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffbdc0bf"/>
-      <rgbColor rgb="ffa5a5a5"/>
+      <rgbColor rgb="ffffffff"/>
+      <rgbColor rgb="ffaaaaaa"/>
       <rgbColor rgb="ff3f3f3f"/>
       <rgbColor rgb="ffdbdbdb"/>
+      <rgbColor rgb="ffa5a5a5"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -226,10 +187,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="5E5E5E"/>
+        <a:srgbClr val="A7A7A7"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="D5D5D5"/>
+        <a:srgbClr val="535353"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -406,11 +367,14 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:srgbClr val="000000"/>
+          <a:srgbClr val="FFFFFF"/>
         </a:solidFill>
-        <a:ln w="12700" cap="flat">
-          <a:noFill/>
-          <a:miter lim="400000"/>
+        <a:ln w="25400" cap="flat">
+          <a:solidFill>
+            <a:schemeClr val="accent1"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -419,33 +383,33 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="584200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="FFFFFF"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="Helvetica Neue Medium"/>
-            <a:ea typeface="Helvetica Neue Medium"/>
-            <a:cs typeface="Helvetica Neue Medium"/>
-            <a:sym typeface="Helvetica Neue Medium"/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="000000"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="+mn-lt"/>
+            <a:ea typeface="+mn-ea"/>
+            <a:cs typeface="+mn-cs"/>
+            <a:sym typeface="Helvetica Neue"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -684,12 +648,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="12700" cap="flat">
+        <a:ln w="25400" cap="flat">
           <a:solidFill>
-            <a:srgbClr val="000000"/>
+            <a:schemeClr val="accent1"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:miter lim="400000"/>
+          <a:round/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -970,7 +934,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1238,122 +1202,87 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="B2:C23"/>
+  <dimension ref="A1:A22"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
-      <pane topLeftCell="C3" xSplit="2" ySplit="2" activePane="bottomRight" state="frozen"/>
-    </sheetView>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="10.4219" style="1" customWidth="1"/>
-    <col min="2" max="2" width="70.3047" style="1" customWidth="1"/>
-    <col min="3" max="3" width="16.3516" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="16.3516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="70.3516" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" ht="27.65" customHeight="1">
-      <c r="B1" t="s" s="2">
+      <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" ht="20.25" customHeight="1">
-      <c r="B2" t="s" s="3">
+    </row>
+    <row r="2" ht="30.2" customHeight="1">
+      <c r="A2" t="s" s="3">
         <v>1</v>
       </c>
-      <c r="C2" s="4"/>
-    </row>
-    <row r="3" ht="30.2" customHeight="1">
-      <c r="B3" t="s" s="5">
-        <v>2</v>
-      </c>
-      <c r="C3" s="6"/>
+    </row>
+    <row r="3" ht="20.05" customHeight="1">
+      <c r="A3" s="4"/>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="B4" s="7"/>
-      <c r="C4" s="8"/>
+      <c r="A4" s="4"/>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="B5" s="7"/>
-      <c r="C5" s="8"/>
+      <c r="A5" s="4"/>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="B6" s="7"/>
-      <c r="C6" s="8"/>
+      <c r="A6" s="4"/>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="B7" s="7"/>
-      <c r="C7" s="8"/>
+      <c r="A7" s="4"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="B8" s="7"/>
-      <c r="C8" s="8"/>
+      <c r="A8" s="4"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="B9" s="7"/>
-      <c r="C9" s="8"/>
+      <c r="A9" s="4"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="B10" s="7"/>
-      <c r="C10" s="8"/>
+      <c r="A10" s="4"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="B11" s="7"/>
-      <c r="C11" s="8"/>
+      <c r="A11" s="4"/>
     </row>
     <row r="12" ht="20.05" customHeight="1">
-      <c r="B12" s="7"/>
-      <c r="C12" s="8"/>
+      <c r="A12" s="4"/>
     </row>
     <row r="13" ht="20.05" customHeight="1">
-      <c r="B13" s="7"/>
-      <c r="C13" s="8"/>
+      <c r="A13" s="4"/>
     </row>
     <row r="14" ht="20.05" customHeight="1">
-      <c r="B14" s="7"/>
-      <c r="C14" s="8"/>
+      <c r="A14" s="4"/>
     </row>
     <row r="15" ht="20.05" customHeight="1">
-      <c r="B15" s="7"/>
-      <c r="C15" s="8"/>
+      <c r="A15" s="4"/>
     </row>
     <row r="16" ht="20.05" customHeight="1">
-      <c r="B16" s="7"/>
-      <c r="C16" s="8"/>
+      <c r="A16" s="4"/>
     </row>
     <row r="17" ht="20.05" customHeight="1">
-      <c r="B17" s="7"/>
-      <c r="C17" s="8"/>
+      <c r="A17" s="4"/>
     </row>
     <row r="18" ht="20.05" customHeight="1">
-      <c r="B18" s="7"/>
-      <c r="C18" s="8"/>
+      <c r="A18" s="4"/>
     </row>
     <row r="19" ht="20.05" customHeight="1">
-      <c r="B19" s="7"/>
-      <c r="C19" s="8"/>
+      <c r="A19" s="4"/>
     </row>
     <row r="20" ht="20.05" customHeight="1">
-      <c r="B20" s="7"/>
-      <c r="C20" s="8"/>
+      <c r="A20" s="4"/>
     </row>
     <row r="21" ht="20.05" customHeight="1">
-      <c r="B21" s="7"/>
-      <c r="C21" s="8"/>
+      <c r="A21" s="4"/>
     </row>
     <row r="22" ht="20.05" customHeight="1">
-      <c r="B22" s="7"/>
-      <c r="C22" s="8"/>
-    </row>
-    <row r="23" ht="20.05" customHeight="1">
-      <c r="B23" s="7"/>
-      <c r="C23" s="8"/>
+      <c r="A22" s="4"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:C1"/>
-  </mergeCells>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>
   <pageSetup firstPageNumber="1" fitToHeight="1" fitToWidth="1" scale="72" useFirstPageNumber="0" orientation="portrait" pageOrder="downThenOver"/>
   <headerFooter>

</xml_diff>

<commit_message>
test(app): fix problems with test case of analyze
</commit_message>
<xml_diff>
--- a/system_tests/data/analyze_tc_1/stories.xlsx
+++ b/system_tests/data/analyze_tc_1/stories.xlsx
@@ -5,7 +5,7 @@
     <workbookView xWindow="0" yWindow="40" windowWidth="15960" windowHeight="18080"/>
   </bookViews>
   <sheets>
-    <sheet name="Foglio 1" sheetId="1" r:id="rId4"/>
+    <sheet name="Foglio 1 - User Story" sheetId="1" r:id="rId4"/>
   </sheets>
 </workbook>
 </file>
@@ -16,7 +16,8 @@
     <t>User Story</t>
   </si>
   <si>
-    <t>A group of researchers is using abstractive summarization to identify key trends and insights in large sets of biological data, enabling more efficient analysis and interpretation.</t>
+    <t xml:space="preserve">As a radiologist, I want to use the ID3 algorithm to develop decision tree models for diagnosing and predicting medical conditions based on various medical imaging data, such as X-rays, CT scans, and MRI scans.
+</t>
   </si>
 </sst>
 </file>
@@ -26,7 +27,7 @@
   <numFmts count="1">
     <numFmt numFmtId="0" formatCode="General"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="3">
     <font>
       <sz val="10"/>
       <color indexed="8"/>
@@ -38,23 +39,12 @@
       <name val="Helvetica Neue"/>
     </font>
     <font>
-      <sz val="15"/>
-      <color indexed="8"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color indexed="8"/>
-      <name val="Arial"/>
-    </font>
-    <font>
-      <b val="1"/>
-      <sz val="10"/>
+      <sz val="11"/>
       <color indexed="8"/>
       <name val="Helvetica Neue"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -64,12 +54,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="9"/>
-        <bgColor auto="1"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="12"/>
         <bgColor auto="1"/>
       </patternFill>
     </fill>
@@ -99,31 +83,31 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
         <color indexed="11"/>
       </top>
       <bottom style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
     <border>
       <left style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </left>
       <right style="thin">
-        <color indexed="11"/>
+        <color indexed="10"/>
       </right>
       <top style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </top>
       <bottom style="thin">
-        <color indexed="13"/>
+        <color indexed="10"/>
       </bottom>
       <diagonal/>
     </border>
@@ -133,20 +117,23 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" applyNumberFormat="1" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="1" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="0" applyAlignment="1" applyProtection="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="3" fillId="3" borderId="2" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="0">
+    <xf numFmtId="0" fontId="0" borderId="2" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" borderId="3" applyNumberFormat="0" applyFont="1" applyFill="0" applyBorder="1" applyAlignment="1" applyProtection="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -166,11 +153,9 @@
       <rgbColor rgb="ffff00ff"/>
       <rgbColor rgb="ff00ffff"/>
       <rgbColor rgb="ff000000"/>
-      <rgbColor rgb="ffffffff"/>
-      <rgbColor rgb="ffaaaaaa"/>
+      <rgbColor rgb="ffbdc0bf"/>
+      <rgbColor rgb="ffa5a5a5"/>
       <rgbColor rgb="ff3f3f3f"/>
-      <rgbColor rgb="ffdbdbdb"/>
-      <rgbColor rgb="ffa5a5a5"/>
     </indexedColors>
   </colors>
 </styleSheet>
@@ -187,10 +172,10 @@
         <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="A7A7A7"/>
+        <a:srgbClr val="5E5E5E"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="535353"/>
+        <a:srgbClr val="D5D5D5"/>
       </a:lt2>
       <a:accent1>
         <a:srgbClr val="00A2FF"/>
@@ -367,14 +352,11 @@
     <a:spDef>
       <a:spPr>
         <a:solidFill>
-          <a:srgbClr val="FFFFFF"/>
+          <a:srgbClr val="000000"/>
         </a:solidFill>
-        <a:ln w="25400" cap="flat">
-          <a:solidFill>
-            <a:schemeClr val="accent1"/>
-          </a:solidFill>
-          <a:prstDash val="solid"/>
-          <a:round/>
+        <a:ln w="12700" cap="flat">
+          <a:noFill/>
+          <a:miter lim="400000"/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -383,33 +365,33 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
-          <a:lnSpc>
-            <a:spcPct val="100000"/>
-          </a:lnSpc>
-          <a:spcBef>
-            <a:spcPts val="0"/>
-          </a:spcBef>
-          <a:spcAft>
-            <a:spcPts val="0"/>
-          </a:spcAft>
-          <a:buClrTx/>
-          <a:buSzTx/>
-          <a:buFontTx/>
-          <a:buNone/>
-          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1100" u="none" kumimoji="0" normalizeH="0">
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:solidFill>
-              <a:srgbClr val="000000"/>
-            </a:solidFill>
-            <a:effectLst/>
-            <a:uFillTx/>
-            <a:latin typeface="+mn-lt"/>
-            <a:ea typeface="+mn-ea"/>
-            <a:cs typeface="+mn-cs"/>
-            <a:sym typeface="Helvetica Neue"/>
+        <a:defPPr marL="0" marR="0" indent="0" algn="ctr" defTabSz="584200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+          <a:lnSpc>
+            <a:spcPct val="100000"/>
+          </a:lnSpc>
+          <a:spcBef>
+            <a:spcPts val="0"/>
+          </a:spcBef>
+          <a:spcAft>
+            <a:spcPts val="0"/>
+          </a:spcAft>
+          <a:buClrTx/>
+          <a:buSzTx/>
+          <a:buFontTx/>
+          <a:buNone/>
+          <a:defRPr b="0" baseline="0" cap="none" i="0" spc="0" strike="noStrike" sz="1200" u="none" kumimoji="0" normalizeH="0">
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:solidFill>
+              <a:srgbClr val="FFFFFF"/>
+            </a:solidFill>
+            <a:effectLst/>
+            <a:uFillTx/>
+            <a:latin typeface="Helvetica Neue Medium"/>
+            <a:ea typeface="Helvetica Neue Medium"/>
+            <a:cs typeface="Helvetica Neue Medium"/>
+            <a:sym typeface="Helvetica Neue Medium"/>
           </a:defRPr>
         </a:defPPr>
         <a:lvl1pPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="1" hangingPunct="0">
@@ -648,12 +630,12 @@
     <a:lnDef>
       <a:spPr>
         <a:noFill/>
-        <a:ln w="25400" cap="flat">
+        <a:ln w="12700" cap="flat">
           <a:solidFill>
-            <a:schemeClr val="accent1"/>
+            <a:srgbClr val="000000"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
-          <a:round/>
+          <a:miter lim="400000"/>
         </a:ln>
         <a:effectLst/>
         <a:sp3d/>
@@ -934,7 +916,7 @@
         <a:spAutoFit/>
       </a:bodyPr>
       <a:lstStyle>
-        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="914400" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
+        <a:defPPr marL="0" marR="0" indent="0" algn="l" defTabSz="457200" rtl="0" fontAlgn="auto" latinLnBrk="0" hangingPunct="0">
           <a:lnSpc>
             <a:spcPct val="100000"/>
           </a:lnSpc>
@@ -1202,13 +1184,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:A22"/>
+  <dimension ref="A2:A23"/>
   <sheetViews>
-    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1"/>
+    <sheetView workbookViewId="0" showGridLines="0" defaultGridColor="1">
+      <pane topLeftCell="A3" xSplit="0" ySplit="2" activePane="bottomLeft" state="frozen"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="16.3333" defaultRowHeight="19.9" customHeight="1" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col min="1" max="1" width="70.3516" style="1" customWidth="1"/>
+    <col min="1" max="1" width="119" style="1" customWidth="1"/>
     <col min="2" max="16384" width="16.3516" style="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1217,70 +1201,73 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" ht="30.2" customHeight="1">
+    <row r="2" ht="44.2" customHeight="1">
       <c r="A2" t="s" s="3">
         <v>1</v>
       </c>
     </row>
-    <row r="3" ht="20.05" customHeight="1">
+    <row r="3" ht="20.25" customHeight="1">
       <c r="A3" s="4"/>
     </row>
     <row r="4" ht="20.05" customHeight="1">
-      <c r="A4" s="4"/>
+      <c r="A4" s="5"/>
     </row>
     <row r="5" ht="20.05" customHeight="1">
-      <c r="A5" s="4"/>
+      <c r="A5" s="5"/>
     </row>
     <row r="6" ht="20.05" customHeight="1">
-      <c r="A6" s="4"/>
+      <c r="A6" s="5"/>
     </row>
     <row r="7" ht="20.05" customHeight="1">
-      <c r="A7" s="4"/>
+      <c r="A7" s="5"/>
     </row>
     <row r="8" ht="20.05" customHeight="1">
-      <c r="A8" s="4"/>
+      <c r="A8" s="5"/>
     </row>
     <row r="9" ht="20.05" customHeight="1">
-      <c r="A9" s="4"/>
+      <c r="A9" s="5"/>
     </row>
     <row r="10" ht="20.05" customHeight="1">
-      <c r="A10" s="4"/>
+      <c r="A10" s="5"/>
     </row>
     <row r="11" ht="20.05" customHeight="1">
-      <c r="A11" s="4"/>
+      <c r="A11" s="5"/>
     </row>
     <row r="12" ht="20.05" customHeight="1">
-      <c r="A12" s="4"/>
+      <c r="A12" s="5"/>
     </row>
     <row r="13" ht="20.05" customHeight="1">
-      <c r="A13" s="4"/>
+      <c r="A13" s="5"/>
     </row>
     <row r="14" ht="20.05" customHeight="1">
-      <c r="A14" s="4"/>
+      <c r="A14" s="5"/>
     </row>
     <row r="15" ht="20.05" customHeight="1">
-      <c r="A15" s="4"/>
+      <c r="A15" s="5"/>
     </row>
     <row r="16" ht="20.05" customHeight="1">
-      <c r="A16" s="4"/>
+      <c r="A16" s="5"/>
     </row>
     <row r="17" ht="20.05" customHeight="1">
-      <c r="A17" s="4"/>
+      <c r="A17" s="5"/>
     </row>
     <row r="18" ht="20.05" customHeight="1">
-      <c r="A18" s="4"/>
+      <c r="A18" s="5"/>
     </row>
     <row r="19" ht="20.05" customHeight="1">
-      <c r="A19" s="4"/>
+      <c r="A19" s="5"/>
     </row>
     <row r="20" ht="20.05" customHeight="1">
-      <c r="A20" s="4"/>
+      <c r="A20" s="5"/>
     </row>
     <row r="21" ht="20.05" customHeight="1">
-      <c r="A21" s="4"/>
+      <c r="A21" s="5"/>
     </row>
     <row r="22" ht="20.05" customHeight="1">
-      <c r="A22" s="4"/>
+      <c r="A22" s="5"/>
+    </row>
+    <row r="23" ht="20.05" customHeight="1">
+      <c r="A23" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.5" right="0.5" top="0.75" bottom="0.75" header="0.277778" footer="0.277778"/>

</xml_diff>